<commit_message>
sum of quantity and pop up for file upload
</commit_message>
<xml_diff>
--- a/data/ptfiles_export.xlsx
+++ b/data/ptfiles_export.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Department</t>
   </si>
@@ -82,31 +82,43 @@
     <t>InvoiceDt</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>3612</t>
-  </si>
-  <si>
-    <t>MZ6015-V5</t>
+    <t>TROUSER</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>SC1</t>
+  </si>
+  <si>
+    <t>4114</t>
   </si>
   <si>
     <t>pcs</t>
   </si>
   <si>
-    <t>BLACK</t>
-  </si>
-  <si>
-    <t>BLACK COFFEE</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>1004032300</t>
+    <t>L. GREY</t>
+  </si>
+  <si>
+    <t>L GREY</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>3333</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>2198</t>
+  </si>
+  <si>
+    <t>2195.00</t>
   </si>
 </sst>
 </file>
@@ -543,34 +555,34 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="R2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="T2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -578,31 +590,34 @@
         <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T3">
         <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T3">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
export image feature implemented
</commit_message>
<xml_diff>
--- a/data/ptfiles_export.xlsx
+++ b/data/ptfiles_export.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Department</t>
   </si>
@@ -82,43 +82,46 @@
     <t>InvoiceDt</t>
   </si>
   <si>
-    <t>TROUSER</t>
+    <t>SHIRT</t>
   </si>
   <si>
     <t>C1</t>
   </si>
   <si>
-    <t>SC1</t>
-  </si>
-  <si>
-    <t>4114</t>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>A 1142/2</t>
+  </si>
+  <si>
+    <t>3612</t>
   </si>
   <si>
     <t>pcs</t>
   </si>
   <si>
-    <t>L. GREY</t>
-  </si>
-  <si>
-    <t>L GREY</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>3333</t>
+    <t>OUTFIT BLACK</t>
+  </si>
+  <si>
+    <t>34/86 CM</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>2222</t>
   </si>
   <si>
     <t>1111</t>
   </si>
   <si>
-    <t>2198</t>
-  </si>
-  <si>
-    <t>2195.00</t>
+    <t>2699.0</t>
   </si>
 </sst>
 </file>
@@ -558,31 +561,28 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G2">
-        <v>42</v>
-      </c>
-      <c r="I2" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="R2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="T2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -590,28 +590,28 @@
         <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G3">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="I3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R3" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
dynamic dropdown in size
</commit_message>
<xml_diff>
--- a/data/ptfiles_export.xlsx
+++ b/data/ptfiles_export.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Department</t>
   </si>
@@ -85,10 +85,10 @@
     <t>TROUSER</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>SC1</t>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>SC3</t>
   </si>
   <si>
     <t>4114</t>
@@ -97,25 +97,16 @@
     <t>pcs</t>
   </si>
   <si>
-    <t>L. GREY</t>
-  </si>
-  <si>
-    <t>L GREY</t>
-  </si>
-  <si>
-    <t>38</t>
+    <t>L.GREY</t>
   </si>
   <si>
     <t>36</t>
   </si>
   <si>
-    <t>3333</t>
-  </si>
-  <si>
-    <t>1111</t>
-  </si>
-  <si>
-    <t>2198</t>
+    <t>4444</t>
+  </si>
+  <si>
+    <t>Supplier4</t>
   </si>
   <si>
     <t>2195.00</t>
@@ -476,7 +467,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -567,56 +558,24 @@
         <v>26</v>
       </c>
       <c r="G2">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I2" t="s">
         <v>27</v>
       </c>
       <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
         <v>29</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" t="s">
         <v>31</v>
       </c>
-      <c r="R2" t="s">
-        <v>33</v>
-      </c>
       <c r="T2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3">
-        <v>27</v>
-      </c>
-      <c r="I3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" t="s">
-        <v>32</v>
-      </c>
-      <c r="R3" t="s">
-        <v>34</v>
-      </c>
-      <c r="T3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add prefix and suffix
</commit_message>
<xml_diff>
--- a/data/ptfiles_export.xlsx
+++ b/data/ptfiles_export.xlsx
@@ -14,17 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
   <si>
     <t>Department</t>
   </si>
   <si>
+    <t>Subcategory</t>
+  </si>
+  <si>
     <t>Category</t>
   </si>
   <si>
-    <t>Subcategory</t>
-  </si>
-  <si>
     <t>Article Number</t>
   </si>
   <si>
@@ -82,13 +82,16 @@
     <t>InvoiceDt</t>
   </si>
   <si>
-    <t>TROUSER</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>4114</t>
+    <t>TROUSERS</t>
+  </si>
+  <si>
+    <t>SC1</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>pb141141ds1cs2ss1</t>
   </si>
   <si>
     <t>pcs</t>
@@ -97,13 +100,13 @@
     <t>L.GREY</t>
   </si>
   <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>2222</t>
-  </si>
-  <si>
-    <t>Supplier2</t>
+    <t>32</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>sup12</t>
   </si>
   <si>
     <t>2195.00</t>
@@ -464,7 +467,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -546,34 +549,148 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="G2">
-        <v>37</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="F3" t="s">
         <v>26</v>
       </c>
-      <c r="J2" t="s">
+      <c r="G3">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
         <v>27</v>
       </c>
-      <c r="L2" t="s">
+      <c r="J3" t="s">
         <v>28</v>
       </c>
-      <c r="N2" t="s">
+      <c r="L3" t="s">
         <v>29</v>
       </c>
-      <c r="R2" t="s">
+      <c r="N3" t="s">
         <v>30</v>
       </c>
-      <c r="T2">
-        <v>1</v>
+      <c r="R3" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4">
+        <v>38</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" t="s">
+        <v>31</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
total wsp and is_image_uploaded
</commit_message>
<xml_diff>
--- a/data/ptfiles_export.xlsx
+++ b/data/ptfiles_export.xlsx
@@ -94,16 +94,16 @@
     <t>pcs</t>
   </si>
   <si>
-    <t>L.GREY</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>2222</t>
-  </si>
-  <si>
-    <t>Supplier2</t>
+    <t>L GREY</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>4444</t>
+  </si>
+  <si>
+    <t>Supplier4</t>
   </si>
   <si>
     <t>2195.00</t>
@@ -555,7 +555,7 @@
         <v>25</v>
       </c>
       <c r="G2">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I2" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
changes as per 1st may
</commit_message>
<xml_diff>
--- a/data/ptfiles_export.xlsx
+++ b/data/ptfiles_export.xlsx
@@ -14,17 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>Department</t>
   </si>
   <si>
+    <t>Subcategory</t>
+  </si>
+  <si>
     <t>Category</t>
   </si>
   <si>
-    <t>Subcategory</t>
-  </si>
-  <si>
     <t>Article Number</t>
   </si>
   <si>
@@ -34,27 +34,27 @@
     <t>UOMName</t>
   </si>
   <si>
+    <t>HSNCode</t>
+  </si>
+  <si>
+    <t>ExtDescription</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>ExtDescription</t>
-  </si>
-  <si>
     <t>Color</t>
   </si>
   <si>
+    <t>Style</t>
+  </si>
+  <si>
     <t>Size</t>
   </si>
   <si>
-    <t>Style</t>
-  </si>
-  <si>
     <t>Brand</t>
   </si>
   <si>
-    <t>HSNCode</t>
-  </si>
-  <si>
     <t>Supplier</t>
   </si>
   <si>
@@ -64,7 +64,7 @@
     <t>ItemId</t>
   </si>
   <si>
-    <t>PurPrice</t>
+    <t>Pur Price</t>
   </si>
   <si>
     <t>ItemMRP</t>
@@ -80,12 +80,69 @@
   </si>
   <si>
     <t>InvoiceDt</t>
+  </si>
+  <si>
+    <t>TROUSER</t>
+  </si>
+  <si>
+    <t>SC3</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>TA4114TRccc</t>
+  </si>
+  <si>
+    <t>pcs</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>L GREY</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>2222</t>
+  </si>
+  <si>
+    <t>Supplier2</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>2195.00</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>336</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -138,11 +195,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,7 +495,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -511,6 +569,165 @@
         <v>21</v>
       </c>
     </row>
+    <row r="2" spans="1:22">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="2">
+        <v>45426</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3">
+        <v>47</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T3">
+        <v>2</v>
+      </c>
+      <c r="U3" t="s">
+        <v>38</v>
+      </c>
+      <c r="V3" s="2">
+        <v>45428</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" t="s">
+        <v>36</v>
+      </c>
+      <c r="T4">
+        <v>3</v>
+      </c>
+      <c r="U4" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" s="2">
+        <v>45432</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
pur price mapping fix
</commit_message>
<xml_diff>
--- a/data/ptfiles_export.xlsx
+++ b/data/ptfiles_export.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Department</t>
   </si>
@@ -85,43 +85,61 @@
     <t>TROUSER</t>
   </si>
   <si>
-    <t>SC3</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>TA4114TRccc</t>
+    <t>SHIRT</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>Sidhhit4114TSRTSR001C1S3</t>
+  </si>
+  <si>
+    <t>suffix3612suffixST34C1S2</t>
   </si>
   <si>
     <t>pcs</t>
   </si>
   <si>
-    <t>11</t>
+    <t>TSR1200987ZZ</t>
   </si>
   <si>
     <t>L GREY</t>
   </si>
   <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>2222</t>
-  </si>
-  <si>
-    <t>Supplier2</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>33</t>
+    <t>OUTFIT BLACK</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>Siddhivinayak Apparel</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>2000</t>
   </si>
   <si>
     <t>2195.00</t>
@@ -130,10 +148,10 @@
     <t>111</t>
   </si>
   <si>
-    <t>222</t>
-  </si>
-  <si>
-    <t>336</t>
+    <t>INVOICE1221</t>
+  </si>
+  <si>
+    <t>INVOICE4533</t>
   </si>
 </sst>
 </file>
@@ -495,7 +513,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -574,158 +592,102 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E2">
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I2">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="M2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="N2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="Q2" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="R2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="T2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="V2" s="2">
-        <v>45426</v>
+        <v>45433</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="I3">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="L3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="M3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="N3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="Q3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="R3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="T3">
         <v>2</v>
       </c>
       <c r="U3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="V3" s="2">
-        <v>45428</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4">
-        <v>48</v>
-      </c>
-      <c r="J4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>35</v>
-      </c>
-      <c r="R4" t="s">
-        <v>36</v>
-      </c>
-      <c r="T4">
-        <v>3</v>
-      </c>
-      <c r="U4" t="s">
-        <v>39</v>
-      </c>
-      <c r="V4" s="2">
-        <v>45432</v>
+        <v>45421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>